<commit_message>
NK2 analysis with food groups
</commit_message>
<xml_diff>
--- a/data/raw/norkost/Norkost 2.xlsx
+++ b/data/raw/norkost/Norkost 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\GitHub\food-consumption\data\raw\norkost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F71A21-7C30-47D3-93A1-90077D3856C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868F8282-4849-43BB-A433-9704E29FD6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-16785" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Fruits and berries</t>
-  </si>
-  <si>
     <t>Vegetables</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Fruits and nuts</t>
   </si>
 </sst>
 </file>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,43 +467,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -539,6 +539,9 @@
         <v>17</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>141</v>
       </c>
       <c r="M2">
@@ -588,6 +591,9 @@
         <v>21</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>141</v>
       </c>
       <c r="M3">
@@ -637,6 +643,9 @@
         <v>20</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>143</v>
       </c>
       <c r="M4">
@@ -686,6 +695,9 @@
         <v>19</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>119</v>
       </c>
       <c r="M5">
@@ -735,6 +747,9 @@
         <v>20</v>
       </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>113</v>
       </c>
       <c r="M6">
@@ -784,6 +799,9 @@
         <v>16</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>96</v>
       </c>
       <c r="M7">
@@ -833,6 +851,9 @@
         <v>17</v>
       </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>96</v>
       </c>
       <c r="M8">
@@ -882,6 +903,9 @@
         <v>11</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>87</v>
       </c>
       <c r="M9">
@@ -931,6 +955,9 @@
         <v>14</v>
       </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>88</v>
       </c>
       <c r="M10">
@@ -980,6 +1007,9 @@
         <v>16</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>94</v>
       </c>
       <c r="M11">
@@ -1029,6 +1059,9 @@
         <v>16</v>
       </c>
       <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>94</v>
       </c>
       <c r="M12">
@@ -1078,6 +1111,9 @@
         <v>16</v>
       </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>86</v>
       </c>
       <c r="M13">
@@ -1127,6 +1163,9 @@
         <v>14</v>
       </c>
       <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>78</v>
       </c>
       <c r="M14">
@@ -1176,6 +1215,9 @@
         <v>16</v>
       </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>65</v>
       </c>
       <c r="M15">

</xml_diff>